<commit_message>
Update MSIS with correct population for Bergen and Stavanger
</commit_message>
<xml_diff>
--- a/data/01_infected/msis/municipality_and_district_wide.xlsx
+++ b/data/01_infected/msis/municipality_and_district_wide.xlsx
@@ -2129,6 +2129,9 @@
           <t>Rogaland</t>
         </is>
       </c>
+      <c r="J21">
+        <v>143574</v>
+      </c>
       <c r="K21">
         <v>87</v>
       </c>
@@ -23876,6 +23879,9 @@
           <t>Trøndelag</t>
         </is>
       </c>
+      <c r="J306">
+        <v>205163</v>
+      </c>
       <c r="K306">
         <v>113</v>
       </c>
@@ -29725,6 +29731,9 @@
           <t>Svalbard</t>
         </is>
       </c>
+      <c r="J383">
+        <v>0</v>
+      </c>
       <c r="K383">
         <v>0</v>
       </c>
@@ -29797,6 +29806,9 @@
         <is>
           <t>Ukjent Fylke</t>
         </is>
+      </c>
+      <c r="J384">
+        <v>0</v>
       </c>
       <c r="K384">
         <v>109</v>

</xml_diff>

<commit_message>
Add Apple Mobility Data
</commit_message>
<xml_diff>
--- a/data/01_infected/msis/municipality_and_district_wide.xlsx
+++ b/data/01_infected/msis/municipality_and_district_wide.xlsx
@@ -351,7 +351,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AD384"/>
+  <dimension ref="A1:AE384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -508,6 +508,11 @@
           <t>2020-04-14</t>
         </is>
       </c>
+      <c r="AE1" s="1" t="inlineStr">
+        <is>
+          <t>2020-04-15</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -618,6 +623,9 @@
       <c r="AD2">
         <v>199</v>
       </c>
+      <c r="AE2">
+        <v>202</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
@@ -728,6 +736,9 @@
       <c r="AD3">
         <v>141</v>
       </c>
+      <c r="AE3">
+        <v>143</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
@@ -838,6 +849,9 @@
       <c r="AD4">
         <v>117</v>
       </c>
+      <c r="AE4">
+        <v>119</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
@@ -948,6 +962,9 @@
       <c r="AD5">
         <v>78</v>
       </c>
+      <c r="AE5">
+        <v>80</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
@@ -1058,6 +1075,9 @@
       <c r="AD6">
         <v>146</v>
       </c>
+      <c r="AE6">
+        <v>148</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
@@ -1168,6 +1188,9 @@
       <c r="AD7">
         <v>104</v>
       </c>
+      <c r="AE7">
+        <v>104</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -1278,6 +1301,9 @@
       <c r="AD8">
         <v>132</v>
       </c>
+      <c r="AE8">
+        <v>135</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
@@ -1388,6 +1414,9 @@
       <c r="AD9">
         <v>117</v>
       </c>
+      <c r="AE9">
+        <v>117</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
@@ -1498,6 +1527,9 @@
       <c r="AD10">
         <v>78</v>
       </c>
+      <c r="AE10">
+        <v>81</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
@@ -1608,6 +1640,9 @@
       <c r="AD11">
         <v>80</v>
       </c>
+      <c r="AE11">
+        <v>80</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
@@ -1718,6 +1753,9 @@
       <c r="AD12">
         <v>143</v>
       </c>
+      <c r="AE12">
+        <v>146</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
@@ -1828,6 +1866,9 @@
       <c r="AD13">
         <v>179</v>
       </c>
+      <c r="AE13">
+        <v>180</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
@@ -1938,6 +1979,9 @@
       <c r="AD14">
         <v>152</v>
       </c>
+      <c r="AE14">
+        <v>153</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
@@ -2048,6 +2092,9 @@
       <c r="AD15">
         <v>139</v>
       </c>
+      <c r="AE15">
+        <v>139</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
@@ -2158,6 +2205,9 @@
       <c r="AD16">
         <v>114</v>
       </c>
+      <c r="AE16">
+        <v>116</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
@@ -2268,6 +2318,9 @@
       <c r="AD17">
         <v>4</v>
       </c>
+      <c r="AE17">
+        <v>4</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
@@ -2378,6 +2431,9 @@
       <c r="AD18">
         <v>2</v>
       </c>
+      <c r="AE18">
+        <v>2</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
@@ -2488,6 +2544,9 @@
       <c r="AD19">
         <v>35</v>
       </c>
+      <c r="AE19">
+        <v>36</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
@@ -2588,6 +2647,9 @@
       <c r="AD20">
         <v>14</v>
       </c>
+      <c r="AE20">
+        <v>14</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
@@ -2688,6 +2750,9 @@
       <c r="AD21">
         <v>125</v>
       </c>
+      <c r="AE21">
+        <v>125</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
@@ -2788,6 +2853,9 @@
       <c r="AD22">
         <v>49</v>
       </c>
+      <c r="AE22">
+        <v>49</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
@@ -2888,6 +2956,9 @@
       <c r="AD23">
         <v>46</v>
       </c>
+      <c r="AE23">
+        <v>46</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
@@ -2988,6 +3059,9 @@
       <c r="AD24">
         <v>3</v>
       </c>
+      <c r="AE24">
+        <v>3</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
@@ -3088,6 +3162,9 @@
       <c r="AD25">
         <v>0</v>
       </c>
+      <c r="AE25">
+        <v>1</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
@@ -3188,6 +3265,9 @@
       <c r="AD26">
         <v>0</v>
       </c>
+      <c r="AE26">
+        <v>0</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
@@ -3288,6 +3368,9 @@
       <c r="AD27">
         <v>6</v>
       </c>
+      <c r="AE27">
+        <v>6</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
@@ -3388,6 +3471,9 @@
       <c r="AD28">
         <v>6</v>
       </c>
+      <c r="AE28">
+        <v>6</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
@@ -3488,6 +3574,9 @@
       <c r="AD29">
         <v>12</v>
       </c>
+      <c r="AE29">
+        <v>12</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
@@ -3588,6 +3677,9 @@
       <c r="AD30">
         <v>12</v>
       </c>
+      <c r="AE30">
+        <v>13</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
@@ -3688,6 +3780,9 @@
       <c r="AD31">
         <v>13</v>
       </c>
+      <c r="AE31">
+        <v>13</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
@@ -3788,6 +3883,9 @@
       <c r="AD32">
         <v>11</v>
       </c>
+      <c r="AE32">
+        <v>11</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
@@ -3888,6 +3986,9 @@
       <c r="AD33">
         <v>13</v>
       </c>
+      <c r="AE33">
+        <v>13</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
@@ -3988,6 +4089,9 @@
       <c r="AD34">
         <v>0</v>
       </c>
+      <c r="AE34">
+        <v>0</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
@@ -4088,6 +4192,9 @@
       <c r="AD35">
         <v>0</v>
       </c>
+      <c r="AE35">
+        <v>0</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
@@ -4188,6 +4295,9 @@
       <c r="AD36">
         <v>3</v>
       </c>
+      <c r="AE36">
+        <v>3</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
@@ -4288,6 +4398,9 @@
       <c r="AD37">
         <v>0</v>
       </c>
+      <c r="AE37">
+        <v>0</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
@@ -4388,6 +4501,9 @@
       <c r="AD38">
         <v>1</v>
       </c>
+      <c r="AE38">
+        <v>1</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
@@ -4488,6 +4604,9 @@
       <c r="AD39">
         <v>20</v>
       </c>
+      <c r="AE39">
+        <v>20</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
@@ -4588,6 +4707,9 @@
       <c r="AD40">
         <v>36</v>
       </c>
+      <c r="AE40">
+        <v>36</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
@@ -4688,6 +4810,9 @@
       <c r="AD41">
         <v>0</v>
       </c>
+      <c r="AE41">
+        <v>0</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
@@ -4788,6 +4913,9 @@
       <c r="AD42">
         <v>11</v>
       </c>
+      <c r="AE42">
+        <v>11</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
@@ -4888,6 +5016,9 @@
       <c r="AD43">
         <v>18</v>
       </c>
+      <c r="AE43">
+        <v>18</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
@@ -4988,6 +5119,9 @@
       <c r="AD44">
         <v>14</v>
       </c>
+      <c r="AE44">
+        <v>14</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
@@ -5088,6 +5222,9 @@
       <c r="AD45">
         <v>26</v>
       </c>
+      <c r="AE45">
+        <v>26</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
@@ -5188,6 +5325,9 @@
       <c r="AD46">
         <v>1</v>
       </c>
+      <c r="AE46">
+        <v>1</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
@@ -5288,6 +5428,9 @@
       <c r="AD47">
         <v>3</v>
       </c>
+      <c r="AE47">
+        <v>3</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
@@ -5388,6 +5531,9 @@
       <c r="AD48">
         <v>3</v>
       </c>
+      <c r="AE48">
+        <v>3</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
@@ -5488,6 +5634,9 @@
       <c r="AD49">
         <v>7</v>
       </c>
+      <c r="AE49">
+        <v>7</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
@@ -5588,6 +5737,9 @@
       <c r="AD50">
         <v>2</v>
       </c>
+      <c r="AE50">
+        <v>2</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
@@ -5688,6 +5840,9 @@
       <c r="AD51">
         <v>6</v>
       </c>
+      <c r="AE51">
+        <v>6</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
@@ -5788,6 +5943,9 @@
       <c r="AD52">
         <v>0</v>
       </c>
+      <c r="AE52">
+        <v>0</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
@@ -5888,6 +6046,9 @@
       <c r="AD53">
         <v>0</v>
       </c>
+      <c r="AE53">
+        <v>0</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
@@ -5988,6 +6149,9 @@
       <c r="AD54">
         <v>6</v>
       </c>
+      <c r="AE54">
+        <v>6</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
@@ -6088,6 +6252,9 @@
       <c r="AD55">
         <v>5</v>
       </c>
+      <c r="AE55">
+        <v>5</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
@@ -6188,6 +6355,9 @@
       <c r="AD56">
         <v>0</v>
       </c>
+      <c r="AE56">
+        <v>0</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
@@ -6288,6 +6458,9 @@
       <c r="AD57">
         <v>10</v>
       </c>
+      <c r="AE57">
+        <v>10</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
@@ -6388,6 +6561,9 @@
       <c r="AD58">
         <v>0</v>
       </c>
+      <c r="AE58">
+        <v>0</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
@@ -6488,6 +6664,9 @@
       <c r="AD59">
         <v>0</v>
       </c>
+      <c r="AE59">
+        <v>0</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
@@ -6588,6 +6767,9 @@
       <c r="AD60">
         <v>0</v>
       </c>
+      <c r="AE60">
+        <v>0</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
@@ -6688,6 +6870,9 @@
       <c r="AD61">
         <v>1</v>
       </c>
+      <c r="AE61">
+        <v>1</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
@@ -6788,6 +6973,9 @@
       <c r="AD62">
         <v>2</v>
       </c>
+      <c r="AE62">
+        <v>2</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
@@ -6888,6 +7076,9 @@
       <c r="AD63">
         <v>2</v>
       </c>
+      <c r="AE63">
+        <v>2</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
@@ -6988,6 +7179,9 @@
       <c r="AD64">
         <v>0</v>
       </c>
+      <c r="AE64">
+        <v>0</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
@@ -7088,6 +7282,9 @@
       <c r="AD65">
         <v>3</v>
       </c>
+      <c r="AE65">
+        <v>3</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
@@ -7188,6 +7385,9 @@
       <c r="AD66">
         <v>4</v>
       </c>
+      <c r="AE66">
+        <v>4</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
@@ -7288,6 +7488,9 @@
       <c r="AD67">
         <v>1</v>
       </c>
+      <c r="AE67">
+        <v>1</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
@@ -7388,6 +7591,9 @@
       <c r="AD68">
         <v>3</v>
       </c>
+      <c r="AE68">
+        <v>3</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
@@ -7488,6 +7694,9 @@
       <c r="AD69">
         <v>34</v>
       </c>
+      <c r="AE69">
+        <v>34</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
@@ -7588,6 +7797,9 @@
       <c r="AD70">
         <v>3</v>
       </c>
+      <c r="AE70">
+        <v>3</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
@@ -7688,6 +7900,9 @@
       <c r="AD71">
         <v>0</v>
       </c>
+      <c r="AE71">
+        <v>0</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
@@ -7788,6 +8003,9 @@
       <c r="AD72">
         <v>2</v>
       </c>
+      <c r="AE72">
+        <v>2</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
@@ -7888,6 +8106,9 @@
       <c r="AD73">
         <v>5</v>
       </c>
+      <c r="AE73">
+        <v>5</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
@@ -7988,6 +8209,9 @@
       <c r="AD74">
         <v>3</v>
       </c>
+      <c r="AE74">
+        <v>3</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
@@ -8088,6 +8312,9 @@
       <c r="AD75">
         <v>0</v>
       </c>
+      <c r="AE75">
+        <v>0</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
@@ -8188,6 +8415,9 @@
       <c r="AD76">
         <v>0</v>
       </c>
+      <c r="AE76">
+        <v>0</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
@@ -8288,6 +8518,9 @@
       <c r="AD77">
         <v>2</v>
       </c>
+      <c r="AE77">
+        <v>2</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
@@ -8388,6 +8621,9 @@
       <c r="AD78">
         <v>3</v>
       </c>
+      <c r="AE78">
+        <v>3</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
@@ -8488,6 +8724,9 @@
       <c r="AD79">
         <v>1</v>
       </c>
+      <c r="AE79">
+        <v>1</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
@@ -8588,6 +8827,9 @@
       <c r="AD80">
         <v>1</v>
       </c>
+      <c r="AE80">
+        <v>1</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
@@ -8688,6 +8930,9 @@
       <c r="AD81">
         <v>0</v>
       </c>
+      <c r="AE81">
+        <v>0</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
@@ -8788,6 +9033,9 @@
       <c r="AD82">
         <v>5</v>
       </c>
+      <c r="AE82">
+        <v>5</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
@@ -8888,6 +9136,9 @@
       <c r="AD83">
         <v>0</v>
       </c>
+      <c r="AE83">
+        <v>0</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
@@ -8988,6 +9239,9 @@
       <c r="AD84">
         <v>0</v>
       </c>
+      <c r="AE84">
+        <v>0</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
@@ -9088,6 +9342,9 @@
       <c r="AD85">
         <v>4</v>
       </c>
+      <c r="AE85">
+        <v>4</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
@@ -9188,6 +9445,9 @@
       <c r="AD86">
         <v>0</v>
       </c>
+      <c r="AE86">
+        <v>0</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
@@ -9288,6 +9548,9 @@
       <c r="AD87">
         <v>0</v>
       </c>
+      <c r="AE87">
+        <v>0</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
@@ -9388,6 +9651,9 @@
       <c r="AD88">
         <v>0</v>
       </c>
+      <c r="AE88">
+        <v>0</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
@@ -9488,6 +9754,9 @@
       <c r="AD89">
         <v>5</v>
       </c>
+      <c r="AE89">
+        <v>5</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
@@ -9588,6 +9857,9 @@
       <c r="AD90">
         <v>0</v>
       </c>
+      <c r="AE90">
+        <v>0</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
@@ -9688,6 +9960,9 @@
       <c r="AD91">
         <v>0</v>
       </c>
+      <c r="AE91">
+        <v>0</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
@@ -9788,6 +10063,9 @@
       <c r="AD92">
         <v>0</v>
       </c>
+      <c r="AE92">
+        <v>0</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
@@ -9888,6 +10166,9 @@
       <c r="AD93">
         <v>1</v>
       </c>
+      <c r="AE93">
+        <v>1</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
@@ -9988,6 +10269,9 @@
       <c r="AD94">
         <v>0</v>
       </c>
+      <c r="AE94">
+        <v>0</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -10088,6 +10372,9 @@
       <c r="AD95">
         <v>1</v>
       </c>
+      <c r="AE95">
+        <v>1</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
@@ -10188,6 +10475,9 @@
       <c r="AD96">
         <v>0</v>
       </c>
+      <c r="AE96">
+        <v>0</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
@@ -10288,6 +10578,9 @@
       <c r="AD97">
         <v>0</v>
       </c>
+      <c r="AE97">
+        <v>0</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
@@ -10388,6 +10681,9 @@
       <c r="AD98">
         <v>0</v>
       </c>
+      <c r="AE98">
+        <v>0</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
@@ -10488,6 +10784,9 @@
       <c r="AD99">
         <v>0</v>
       </c>
+      <c r="AE99">
+        <v>0</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
@@ -10588,6 +10887,9 @@
       <c r="AD100">
         <v>4</v>
       </c>
+      <c r="AE100">
+        <v>4</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
@@ -10688,6 +10990,9 @@
       <c r="AD101">
         <v>7</v>
       </c>
+      <c r="AE101">
+        <v>9</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
@@ -10788,6 +11093,9 @@
       <c r="AD102">
         <v>3</v>
       </c>
+      <c r="AE102">
+        <v>3</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
@@ -10888,6 +11196,9 @@
       <c r="AD103">
         <v>5</v>
       </c>
+      <c r="AE103">
+        <v>5</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104" t="inlineStr">
@@ -10988,6 +11299,9 @@
       <c r="AD104">
         <v>0</v>
       </c>
+      <c r="AE104">
+        <v>0</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105" t="inlineStr">
@@ -11088,6 +11402,9 @@
       <c r="AD105">
         <v>0</v>
       </c>
+      <c r="AE105">
+        <v>0</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106" t="inlineStr">
@@ -11188,6 +11505,9 @@
       <c r="AD106">
         <v>6</v>
       </c>
+      <c r="AE106">
+        <v>6</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107" t="inlineStr">
@@ -11288,6 +11608,9 @@
       <c r="AD107">
         <v>0</v>
       </c>
+      <c r="AE107">
+        <v>0</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108" t="inlineStr">
@@ -11388,6 +11711,9 @@
       <c r="AD108">
         <v>0</v>
       </c>
+      <c r="AE108">
+        <v>0</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109" t="inlineStr">
@@ -11488,6 +11814,9 @@
       <c r="AD109">
         <v>0</v>
       </c>
+      <c r="AE109">
+        <v>0</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110" t="inlineStr">
@@ -11588,6 +11917,9 @@
       <c r="AD110">
         <v>28</v>
       </c>
+      <c r="AE110">
+        <v>28</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111" t="inlineStr">
@@ -11688,6 +12020,9 @@
       <c r="AD111">
         <v>85</v>
       </c>
+      <c r="AE111">
+        <v>89</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112" t="inlineStr">
@@ -11788,6 +12123,9 @@
       <c r="AD112">
         <v>54</v>
       </c>
+      <c r="AE112">
+        <v>53</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113" t="inlineStr">
@@ -11888,6 +12226,9 @@
       <c r="AD113">
         <v>74</v>
       </c>
+      <c r="AE113">
+        <v>79</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114" t="inlineStr">
@@ -11988,6 +12329,9 @@
       <c r="AD114">
         <v>155</v>
       </c>
+      <c r="AE114">
+        <v>156</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115" t="inlineStr">
@@ -12088,6 +12432,9 @@
       <c r="AD115">
         <v>20</v>
       </c>
+      <c r="AE115">
+        <v>20</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="inlineStr">
@@ -12188,6 +12535,9 @@
       <c r="AD116">
         <v>9</v>
       </c>
+      <c r="AE116">
+        <v>9</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="inlineStr">
@@ -12288,6 +12638,9 @@
       <c r="AD117">
         <v>2</v>
       </c>
+      <c r="AE117">
+        <v>2</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118" t="inlineStr">
@@ -12388,6 +12741,9 @@
       <c r="AD118">
         <v>2</v>
       </c>
+      <c r="AE118">
+        <v>2</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
@@ -12488,6 +12844,9 @@
       <c r="AD119">
         <v>3</v>
       </c>
+      <c r="AE119">
+        <v>3</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120" t="inlineStr">
@@ -12588,6 +12947,9 @@
       <c r="AD120">
         <v>45</v>
       </c>
+      <c r="AE120">
+        <v>45</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121" t="inlineStr">
@@ -12688,6 +13050,9 @@
       <c r="AD121">
         <v>2</v>
       </c>
+      <c r="AE121">
+        <v>2</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122" t="inlineStr">
@@ -12788,6 +13153,9 @@
       <c r="AD122">
         <v>1</v>
       </c>
+      <c r="AE122">
+        <v>1</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123" t="inlineStr">
@@ -12888,6 +13256,9 @@
       <c r="AD123">
         <v>2</v>
       </c>
+      <c r="AE123">
+        <v>2</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124" t="inlineStr">
@@ -12988,6 +13359,9 @@
       <c r="AD124">
         <v>6</v>
       </c>
+      <c r="AE124">
+        <v>6</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
@@ -13088,6 +13462,9 @@
       <c r="AD125">
         <v>22</v>
       </c>
+      <c r="AE125">
+        <v>22</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
@@ -13188,6 +13565,9 @@
       <c r="AD126">
         <v>89</v>
       </c>
+      <c r="AE126">
+        <v>89</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127" t="inlineStr">
@@ -13288,6 +13668,9 @@
       <c r="AD127">
         <v>17</v>
       </c>
+      <c r="AE127">
+        <v>17</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128" t="inlineStr">
@@ -13388,6 +13771,9 @@
       <c r="AD128">
         <v>18</v>
       </c>
+      <c r="AE128">
+        <v>18</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
@@ -13488,6 +13874,9 @@
       <c r="AD129">
         <v>44</v>
       </c>
+      <c r="AE129">
+        <v>44</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
@@ -13588,6 +13977,9 @@
       <c r="AD130">
         <v>373</v>
       </c>
+      <c r="AE130">
+        <v>383</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
@@ -13688,6 +14080,9 @@
       <c r="AD131">
         <v>152</v>
       </c>
+      <c r="AE131">
+        <v>153</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
@@ -13788,6 +14183,9 @@
       <c r="AD132">
         <v>8</v>
       </c>
+      <c r="AE132">
+        <v>8</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
@@ -13888,6 +14286,9 @@
       <c r="AD133">
         <v>19</v>
       </c>
+      <c r="AE133">
+        <v>21</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
@@ -13988,6 +14389,9 @@
       <c r="AD134">
         <v>43</v>
       </c>
+      <c r="AE134">
+        <v>43</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
@@ -14088,6 +14492,9 @@
       <c r="AD135">
         <v>76</v>
       </c>
+      <c r="AE135">
+        <v>76</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136" t="inlineStr">
@@ -14188,6 +14595,9 @@
       <c r="AD136">
         <v>134</v>
       </c>
+      <c r="AE136">
+        <v>135</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="inlineStr">
@@ -14288,6 +14698,9 @@
       <c r="AD137">
         <v>45</v>
       </c>
+      <c r="AE137">
+        <v>45</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
@@ -14388,6 +14801,9 @@
       <c r="AD138">
         <v>8</v>
       </c>
+      <c r="AE138">
+        <v>8</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
@@ -14488,6 +14904,9 @@
       <c r="AD139">
         <v>52</v>
       </c>
+      <c r="AE139">
+        <v>52</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
@@ -14588,6 +15007,9 @@
       <c r="AD140">
         <v>13</v>
       </c>
+      <c r="AE140">
+        <v>13</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
@@ -14688,6 +15110,9 @@
       <c r="AD141">
         <v>29</v>
       </c>
+      <c r="AE141">
+        <v>30</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
@@ -14788,6 +15213,9 @@
       <c r="AD142">
         <v>17</v>
       </c>
+      <c r="AE142">
+        <v>17</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
@@ -14888,6 +15316,9 @@
       <c r="AD143">
         <v>2</v>
       </c>
+      <c r="AE143">
+        <v>2</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
@@ -14988,6 +15419,9 @@
       <c r="AD144">
         <v>10</v>
       </c>
+      <c r="AE144">
+        <v>10</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
@@ -15088,6 +15522,9 @@
       <c r="AD145">
         <v>1</v>
       </c>
+      <c r="AE145">
+        <v>1</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
@@ -15188,6 +15625,9 @@
       <c r="AD146">
         <v>7</v>
       </c>
+      <c r="AE146">
+        <v>7</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
@@ -15288,6 +15728,9 @@
       <c r="AD147">
         <v>10</v>
       </c>
+      <c r="AE147">
+        <v>10</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
@@ -15388,6 +15831,9 @@
       <c r="AD148">
         <v>8</v>
       </c>
+      <c r="AE148">
+        <v>8</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
@@ -15488,6 +15934,9 @@
       <c r="AD149">
         <v>13</v>
       </c>
+      <c r="AE149">
+        <v>13</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
@@ -15588,6 +16037,9 @@
       <c r="AD150">
         <v>44</v>
       </c>
+      <c r="AE150">
+        <v>44</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
@@ -15688,6 +16140,9 @@
       <c r="AD151">
         <v>0</v>
       </c>
+      <c r="AE151">
+        <v>0</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
@@ -15788,6 +16243,9 @@
       <c r="AD152">
         <v>0</v>
       </c>
+      <c r="AE152">
+        <v>0</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
@@ -15888,6 +16346,9 @@
       <c r="AD153">
         <v>10</v>
       </c>
+      <c r="AE153">
+        <v>10</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
@@ -15988,6 +16449,9 @@
       <c r="AD154">
         <v>5</v>
       </c>
+      <c r="AE154">
+        <v>5</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
@@ -16088,6 +16552,9 @@
       <c r="AD155">
         <v>32</v>
       </c>
+      <c r="AE155">
+        <v>32</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
@@ -16188,6 +16655,9 @@
       <c r="AD156">
         <v>3</v>
       </c>
+      <c r="AE156">
+        <v>4</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
@@ -16288,6 +16758,9 @@
       <c r="AD157">
         <v>1</v>
       </c>
+      <c r="AE157">
+        <v>1</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
@@ -16388,6 +16861,9 @@
       <c r="AD158">
         <v>2</v>
       </c>
+      <c r="AE158">
+        <v>2</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
@@ -16488,6 +16964,9 @@
       <c r="AD159">
         <v>6</v>
       </c>
+      <c r="AE159">
+        <v>6</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
@@ -16588,6 +17067,9 @@
       <c r="AD160">
         <v>9</v>
       </c>
+      <c r="AE160">
+        <v>9</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
@@ -16688,6 +17170,9 @@
       <c r="AD161">
         <v>1</v>
       </c>
+      <c r="AE161">
+        <v>1</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162" t="inlineStr">
@@ -16788,6 +17273,9 @@
       <c r="AD162">
         <v>78</v>
       </c>
+      <c r="AE162">
+        <v>79</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163" t="inlineStr">
@@ -16888,6 +17376,9 @@
       <c r="AD163">
         <v>32</v>
       </c>
+      <c r="AE163">
+        <v>32</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164" t="inlineStr">
@@ -16988,6 +17479,9 @@
       <c r="AD164">
         <v>15</v>
       </c>
+      <c r="AE164">
+        <v>15</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="inlineStr">
@@ -17088,6 +17582,9 @@
       <c r="AD165">
         <v>57</v>
       </c>
+      <c r="AE165">
+        <v>57</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166" t="inlineStr">
@@ -17188,6 +17685,9 @@
       <c r="AD166">
         <v>11</v>
       </c>
+      <c r="AE166">
+        <v>11</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="inlineStr">
@@ -17288,6 +17788,9 @@
       <c r="AD167">
         <v>33</v>
       </c>
+      <c r="AE167">
+        <v>33</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168" t="inlineStr">
@@ -17388,6 +17891,9 @@
       <c r="AD168">
         <v>0</v>
       </c>
+      <c r="AE168">
+        <v>0</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169" t="inlineStr">
@@ -17488,6 +17994,9 @@
       <c r="AD169">
         <v>17</v>
       </c>
+      <c r="AE169">
+        <v>17</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170" t="inlineStr">
@@ -17588,6 +18097,9 @@
       <c r="AD170">
         <v>4</v>
       </c>
+      <c r="AE170">
+        <v>4</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171" t="inlineStr">
@@ -17688,6 +18200,9 @@
       <c r="AD171">
         <v>5</v>
       </c>
+      <c r="AE171">
+        <v>5</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="inlineStr">
@@ -17788,6 +18303,9 @@
       <c r="AD172">
         <v>3</v>
       </c>
+      <c r="AE172">
+        <v>3</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173" t="inlineStr">
@@ -17888,6 +18406,9 @@
       <c r="AD173">
         <v>3</v>
       </c>
+      <c r="AE173">
+        <v>3</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174" t="inlineStr">
@@ -17988,6 +18509,9 @@
       <c r="AD174">
         <v>15</v>
       </c>
+      <c r="AE174">
+        <v>15</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175" t="inlineStr">
@@ -18088,6 +18612,9 @@
       <c r="AD175">
         <v>2</v>
       </c>
+      <c r="AE175">
+        <v>2</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176" t="inlineStr">
@@ -18188,6 +18715,9 @@
       <c r="AD176">
         <v>4</v>
       </c>
+      <c r="AE176">
+        <v>4</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177" t="inlineStr">
@@ -18288,6 +18818,9 @@
       <c r="AD177">
         <v>0</v>
       </c>
+      <c r="AE177">
+        <v>0</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178" t="inlineStr">
@@ -18388,6 +18921,9 @@
       <c r="AD178">
         <v>0</v>
       </c>
+      <c r="AE178">
+        <v>0</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179" t="inlineStr">
@@ -18488,6 +19024,9 @@
       <c r="AD179">
         <v>2</v>
       </c>
+      <c r="AE179">
+        <v>2</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="inlineStr">
@@ -18588,6 +19127,9 @@
       <c r="AD180">
         <v>0</v>
       </c>
+      <c r="AE180">
+        <v>0</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="inlineStr">
@@ -18688,6 +19230,9 @@
       <c r="AD181">
         <v>0</v>
       </c>
+      <c r="AE181">
+        <v>0</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182" t="inlineStr">
@@ -18788,6 +19333,9 @@
       <c r="AD182">
         <v>1</v>
       </c>
+      <c r="AE182">
+        <v>1</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="inlineStr">
@@ -18888,6 +19436,9 @@
       <c r="AD183">
         <v>0</v>
       </c>
+      <c r="AE183">
+        <v>0</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="inlineStr">
@@ -18988,6 +19539,9 @@
       <c r="AD184">
         <v>1</v>
       </c>
+      <c r="AE184">
+        <v>1</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="inlineStr">
@@ -19088,6 +19642,9 @@
       <c r="AD185">
         <v>5</v>
       </c>
+      <c r="AE185">
+        <v>5</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="inlineStr">
@@ -19188,6 +19745,9 @@
       <c r="AD186">
         <v>2</v>
       </c>
+      <c r="AE186">
+        <v>2</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187" t="inlineStr">
@@ -19288,6 +19848,9 @@
       <c r="AD187">
         <v>1</v>
       </c>
+      <c r="AE187">
+        <v>1</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188" t="inlineStr">
@@ -19388,6 +19951,9 @@
       <c r="AD188">
         <v>3</v>
       </c>
+      <c r="AE188">
+        <v>3</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189" t="inlineStr">
@@ -19488,6 +20054,9 @@
       <c r="AD189">
         <v>2</v>
       </c>
+      <c r="AE189">
+        <v>2</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190" t="inlineStr">
@@ -19588,6 +20157,9 @@
       <c r="AD190">
         <v>13</v>
       </c>
+      <c r="AE190">
+        <v>13</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="inlineStr">
@@ -19688,6 +20260,9 @@
       <c r="AD191">
         <v>36</v>
       </c>
+      <c r="AE191">
+        <v>36</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192" t="inlineStr">
@@ -19788,6 +20363,9 @@
       <c r="AD192">
         <v>1</v>
       </c>
+      <c r="AE192">
+        <v>1</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193" t="inlineStr">
@@ -19888,6 +20466,9 @@
       <c r="AD193">
         <v>8</v>
       </c>
+      <c r="AE193">
+        <v>8</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194" t="inlineStr">
@@ -19988,6 +20569,9 @@
       <c r="AD194">
         <v>2</v>
       </c>
+      <c r="AE194">
+        <v>2</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195" t="inlineStr">
@@ -20088,6 +20672,9 @@
       <c r="AD195">
         <v>5</v>
       </c>
+      <c r="AE195">
+        <v>5</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196" t="inlineStr">
@@ -20188,6 +20775,9 @@
       <c r="AD196">
         <v>4</v>
       </c>
+      <c r="AE196">
+        <v>4</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="inlineStr">
@@ -20288,6 +20878,9 @@
       <c r="AD197">
         <v>10</v>
       </c>
+      <c r="AE197">
+        <v>10</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="inlineStr">
@@ -20388,6 +20981,9 @@
       <c r="AD198">
         <v>9</v>
       </c>
+      <c r="AE198">
+        <v>9</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199" t="inlineStr">
@@ -20488,6 +21084,9 @@
       <c r="AD199">
         <v>2</v>
       </c>
+      <c r="AE199">
+        <v>2</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200" t="inlineStr">
@@ -20588,6 +21187,9 @@
       <c r="AD200">
         <v>1</v>
       </c>
+      <c r="AE200">
+        <v>1</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201" t="inlineStr">
@@ -20688,6 +21290,9 @@
       <c r="AD201">
         <v>0</v>
       </c>
+      <c r="AE201">
+        <v>0</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="inlineStr">
@@ -20788,6 +21393,9 @@
       <c r="AD202">
         <v>1</v>
       </c>
+      <c r="AE202">
+        <v>1</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203" t="inlineStr">
@@ -20888,6 +21496,9 @@
       <c r="AD203">
         <v>9</v>
       </c>
+      <c r="AE203">
+        <v>9</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204" t="inlineStr">
@@ -20988,6 +21599,9 @@
       <c r="AD204">
         <v>0</v>
       </c>
+      <c r="AE204">
+        <v>0</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205" t="inlineStr">
@@ -21088,6 +21702,9 @@
       <c r="AD205">
         <v>0</v>
       </c>
+      <c r="AE205">
+        <v>0</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="inlineStr">
@@ -21188,6 +21805,9 @@
       <c r="AD206">
         <v>0</v>
       </c>
+      <c r="AE206">
+        <v>0</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="inlineStr">
@@ -21288,6 +21908,9 @@
       <c r="AD207">
         <v>24</v>
       </c>
+      <c r="AE207">
+        <v>24</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="inlineStr">
@@ -21388,6 +22011,9 @@
       <c r="AD208">
         <v>18</v>
       </c>
+      <c r="AE208">
+        <v>18</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209" t="inlineStr">
@@ -21488,6 +22114,9 @@
       <c r="AD209">
         <v>55</v>
       </c>
+      <c r="AE209">
+        <v>55</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210" t="inlineStr">
@@ -21588,6 +22217,9 @@
       <c r="AD210">
         <v>37</v>
       </c>
+      <c r="AE210">
+        <v>37</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211" t="inlineStr">
@@ -21688,6 +22320,9 @@
       <c r="AD211">
         <v>28</v>
       </c>
+      <c r="AE211">
+        <v>28</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="inlineStr">
@@ -21788,6 +22423,9 @@
       <c r="AD212">
         <v>8</v>
       </c>
+      <c r="AE212">
+        <v>9</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213" t="inlineStr">
@@ -21888,6 +22526,9 @@
       <c r="AD213">
         <v>38</v>
       </c>
+      <c r="AE213">
+        <v>39</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="inlineStr">
@@ -21988,6 +22629,9 @@
       <c r="AD214">
         <v>4</v>
       </c>
+      <c r="AE214">
+        <v>4</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215" t="inlineStr">
@@ -22088,6 +22732,9 @@
       <c r="AD215">
         <v>21</v>
       </c>
+      <c r="AE215">
+        <v>21</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216" t="inlineStr">
@@ -22188,6 +22835,9 @@
       <c r="AD216">
         <v>2</v>
       </c>
+      <c r="AE216">
+        <v>2</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217" t="inlineStr">
@@ -22288,6 +22938,9 @@
       <c r="AD217">
         <v>5</v>
       </c>
+      <c r="AE217">
+        <v>5</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218" t="inlineStr">
@@ -22388,6 +23041,9 @@
       <c r="AD218">
         <v>1</v>
       </c>
+      <c r="AE218">
+        <v>2</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219" t="inlineStr">
@@ -22488,6 +23144,9 @@
       <c r="AD219">
         <v>1</v>
       </c>
+      <c r="AE219">
+        <v>1</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220" t="inlineStr">
@@ -22588,6 +23247,9 @@
       <c r="AD220">
         <v>2</v>
       </c>
+      <c r="AE220">
+        <v>2</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" t="inlineStr">
@@ -22688,6 +23350,9 @@
       <c r="AD221">
         <v>0</v>
       </c>
+      <c r="AE221">
+        <v>0</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222" t="inlineStr">
@@ -22788,6 +23453,9 @@
       <c r="AD222">
         <v>1</v>
       </c>
+      <c r="AE222">
+        <v>1</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="inlineStr">
@@ -22888,6 +23556,9 @@
       <c r="AD223">
         <v>0</v>
       </c>
+      <c r="AE223">
+        <v>0</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224" t="inlineStr">
@@ -22988,6 +23659,9 @@
       <c r="AD224">
         <v>0</v>
       </c>
+      <c r="AE224">
+        <v>0</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225" t="inlineStr">
@@ -23088,6 +23762,9 @@
       <c r="AD225">
         <v>0</v>
       </c>
+      <c r="AE225">
+        <v>0</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226" t="inlineStr">
@@ -23188,6 +23865,9 @@
       <c r="AD226">
         <v>0</v>
       </c>
+      <c r="AE226">
+        <v>0</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="inlineStr">
@@ -23288,6 +23968,9 @@
       <c r="AD227">
         <v>0</v>
       </c>
+      <c r="AE227">
+        <v>0</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228" t="inlineStr">
@@ -23388,6 +24071,9 @@
       <c r="AD228">
         <v>0</v>
       </c>
+      <c r="AE228">
+        <v>0</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229" t="inlineStr">
@@ -23488,6 +24174,9 @@
       <c r="AD229">
         <v>2</v>
       </c>
+      <c r="AE229">
+        <v>2</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="inlineStr">
@@ -23588,6 +24277,9 @@
       <c r="AD230">
         <v>0</v>
       </c>
+      <c r="AE230">
+        <v>0</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="inlineStr">
@@ -23688,6 +24380,9 @@
       <c r="AD231">
         <v>1</v>
       </c>
+      <c r="AE231">
+        <v>1</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232" t="inlineStr">
@@ -23788,6 +24483,9 @@
       <c r="AD232">
         <v>26</v>
       </c>
+      <c r="AE232">
+        <v>26</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233" t="inlineStr">
@@ -23888,6 +24586,9 @@
       <c r="AD233">
         <v>180</v>
       </c>
+      <c r="AE233">
+        <v>182</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234" t="inlineStr">
@@ -23988,6 +24689,9 @@
       <c r="AD234">
         <v>9</v>
       </c>
+      <c r="AE234">
+        <v>9</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235" t="inlineStr">
@@ -24088,6 +24792,9 @@
       <c r="AD235">
         <v>11</v>
       </c>
+      <c r="AE235">
+        <v>11</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236" t="inlineStr">
@@ -24188,6 +24895,9 @@
       <c r="AD236">
         <v>0</v>
       </c>
+      <c r="AE236">
+        <v>0</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237" t="inlineStr">
@@ -24288,6 +24998,9 @@
       <c r="AD237">
         <v>2</v>
       </c>
+      <c r="AE237">
+        <v>2</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238" t="inlineStr">
@@ -24388,6 +25101,9 @@
       <c r="AD238">
         <v>0</v>
       </c>
+      <c r="AE238">
+        <v>0</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="inlineStr">
@@ -24488,6 +25204,9 @@
       <c r="AD239">
         <v>0</v>
       </c>
+      <c r="AE239">
+        <v>0</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="inlineStr">
@@ -24588,6 +25307,9 @@
       <c r="AD240">
         <v>2</v>
       </c>
+      <c r="AE240">
+        <v>2</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241" t="inlineStr">
@@ -24688,6 +25410,9 @@
       <c r="AD241">
         <v>7</v>
       </c>
+      <c r="AE241">
+        <v>7</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242" t="inlineStr">
@@ -24788,6 +25513,9 @@
       <c r="AD242">
         <v>3</v>
       </c>
+      <c r="AE242">
+        <v>3</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243" t="inlineStr">
@@ -24888,6 +25616,9 @@
       <c r="AD243">
         <v>1</v>
       </c>
+      <c r="AE243">
+        <v>1</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244" t="inlineStr">
@@ -24988,6 +25719,9 @@
       <c r="AD244">
         <v>1</v>
       </c>
+      <c r="AE244">
+        <v>1</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245" t="inlineStr">
@@ -25088,6 +25822,9 @@
       <c r="AD245">
         <v>2</v>
       </c>
+      <c r="AE245">
+        <v>2</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246" t="inlineStr">
@@ -25188,6 +25925,9 @@
       <c r="AD246">
         <v>2</v>
       </c>
+      <c r="AE246">
+        <v>2</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247" t="inlineStr">
@@ -25288,6 +26028,9 @@
       <c r="AD247">
         <v>0</v>
       </c>
+      <c r="AE247">
+        <v>0</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248" t="inlineStr">
@@ -25388,6 +26131,9 @@
       <c r="AD248">
         <v>3</v>
       </c>
+      <c r="AE248">
+        <v>3</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249" t="inlineStr">
@@ -25488,6 +26234,9 @@
       <c r="AD249">
         <v>9</v>
       </c>
+      <c r="AE249">
+        <v>9</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250" t="inlineStr">
@@ -25588,6 +26337,9 @@
       <c r="AD250">
         <v>0</v>
       </c>
+      <c r="AE250">
+        <v>0</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251" t="inlineStr">
@@ -25688,6 +26440,9 @@
       <c r="AD251">
         <v>4</v>
       </c>
+      <c r="AE251">
+        <v>4</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252" t="inlineStr">
@@ -25788,6 +26543,9 @@
       <c r="AD252">
         <v>1</v>
       </c>
+      <c r="AE252">
+        <v>1</v>
+      </c>
     </row>
     <row r="253">
       <c r="A253" t="inlineStr">
@@ -25888,6 +26646,9 @@
       <c r="AD253">
         <v>1</v>
       </c>
+      <c r="AE253">
+        <v>1</v>
+      </c>
     </row>
     <row r="254">
       <c r="A254" t="inlineStr">
@@ -25988,6 +26749,9 @@
       <c r="AD254">
         <v>1</v>
       </c>
+      <c r="AE254">
+        <v>1</v>
+      </c>
     </row>
     <row r="255">
       <c r="A255" t="inlineStr">
@@ -26098,6 +26862,9 @@
       <c r="AD255">
         <v>12</v>
       </c>
+      <c r="AE255">
+        <v>12</v>
+      </c>
     </row>
     <row r="256">
       <c r="A256" t="inlineStr">
@@ -26208,6 +26975,9 @@
       <c r="AD256">
         <v>64</v>
       </c>
+      <c r="AE256">
+        <v>72</v>
+      </c>
     </row>
     <row r="257">
       <c r="A257" t="inlineStr">
@@ -26318,6 +27088,9 @@
       <c r="AD257">
         <v>50</v>
       </c>
+      <c r="AE257">
+        <v>50</v>
+      </c>
     </row>
     <row r="258">
       <c r="A258" t="inlineStr">
@@ -26428,6 +27201,9 @@
       <c r="AD258">
         <v>53</v>
       </c>
+      <c r="AE258">
+        <v>56</v>
+      </c>
     </row>
     <row r="259">
       <c r="A259" t="inlineStr">
@@ -26538,6 +27314,9 @@
       <c r="AD259">
         <v>53</v>
       </c>
+      <c r="AE259">
+        <v>55</v>
+      </c>
     </row>
     <row r="260">
       <c r="A260" t="inlineStr">
@@ -26648,6 +27427,9 @@
       <c r="AD260">
         <v>36</v>
       </c>
+      <c r="AE260">
+        <v>38</v>
+      </c>
     </row>
     <row r="261">
       <c r="A261" t="inlineStr">
@@ -26758,6 +27540,9 @@
       <c r="AD261">
         <v>79</v>
       </c>
+      <c r="AE261">
+        <v>83</v>
+      </c>
     </row>
     <row r="262">
       <c r="A262" t="inlineStr">
@@ -26868,6 +27653,9 @@
       <c r="AD262">
         <v>43</v>
       </c>
+      <c r="AE262">
+        <v>46</v>
+      </c>
     </row>
     <row r="263">
       <c r="A263" t="inlineStr">
@@ -26978,6 +27766,9 @@
       <c r="AD263">
         <v>47</v>
       </c>
+      <c r="AE263">
+        <v>51</v>
+      </c>
     </row>
     <row r="264">
       <c r="A264" t="inlineStr">
@@ -27078,6 +27869,9 @@
       <c r="AD264">
         <v>8</v>
       </c>
+      <c r="AE264">
+        <v>8</v>
+      </c>
     </row>
     <row r="265">
       <c r="A265" t="inlineStr">
@@ -27178,6 +27972,9 @@
       <c r="AD265">
         <v>4</v>
       </c>
+      <c r="AE265">
+        <v>4</v>
+      </c>
     </row>
     <row r="266">
       <c r="A266" t="inlineStr">
@@ -27278,6 +28075,9 @@
       <c r="AD266">
         <v>4</v>
       </c>
+      <c r="AE266">
+        <v>4</v>
+      </c>
     </row>
     <row r="267">
       <c r="A267" t="inlineStr">
@@ -27378,6 +28178,9 @@
       <c r="AD267">
         <v>4</v>
       </c>
+      <c r="AE267">
+        <v>4</v>
+      </c>
     </row>
     <row r="268">
       <c r="A268" t="inlineStr">
@@ -27478,6 +28281,9 @@
       <c r="AD268">
         <v>6</v>
       </c>
+      <c r="AE268">
+        <v>6</v>
+      </c>
     </row>
     <row r="269">
       <c r="A269" t="inlineStr">
@@ -27578,6 +28384,9 @@
       <c r="AD269">
         <v>8</v>
       </c>
+      <c r="AE269">
+        <v>8</v>
+      </c>
     </row>
     <row r="270">
       <c r="A270" t="inlineStr">
@@ -27678,6 +28487,9 @@
       <c r="AD270">
         <v>0</v>
       </c>
+      <c r="AE270">
+        <v>0</v>
+      </c>
     </row>
     <row r="271">
       <c r="A271" t="inlineStr">
@@ -27778,6 +28590,9 @@
       <c r="AD271">
         <v>4</v>
       </c>
+      <c r="AE271">
+        <v>4</v>
+      </c>
     </row>
     <row r="272">
       <c r="A272" t="inlineStr">
@@ -27878,6 +28693,9 @@
       <c r="AD272">
         <v>0</v>
       </c>
+      <c r="AE272">
+        <v>0</v>
+      </c>
     </row>
     <row r="273">
       <c r="A273" t="inlineStr">
@@ -27978,6 +28796,9 @@
       <c r="AD273">
         <v>0</v>
       </c>
+      <c r="AE273">
+        <v>0</v>
+      </c>
     </row>
     <row r="274">
       <c r="A274" t="inlineStr">
@@ -28078,6 +28899,9 @@
       <c r="AD274">
         <v>2</v>
       </c>
+      <c r="AE274">
+        <v>2</v>
+      </c>
     </row>
     <row r="275">
       <c r="A275" t="inlineStr">
@@ -28178,6 +29002,9 @@
       <c r="AD275">
         <v>24</v>
       </c>
+      <c r="AE275">
+        <v>24</v>
+      </c>
     </row>
     <row r="276">
       <c r="A276" t="inlineStr">
@@ -28278,6 +29105,9 @@
       <c r="AD276">
         <v>9</v>
       </c>
+      <c r="AE276">
+        <v>9</v>
+      </c>
     </row>
     <row r="277">
       <c r="A277" t="inlineStr">
@@ -28378,6 +29208,9 @@
       <c r="AD277">
         <v>0</v>
       </c>
+      <c r="AE277">
+        <v>0</v>
+      </c>
     </row>
     <row r="278">
       <c r="A278" t="inlineStr">
@@ -28478,6 +29311,9 @@
       <c r="AD278">
         <v>17</v>
       </c>
+      <c r="AE278">
+        <v>17</v>
+      </c>
     </row>
     <row r="279">
       <c r="A279" t="inlineStr">
@@ -28578,6 +29414,9 @@
       <c r="AD279">
         <v>4</v>
       </c>
+      <c r="AE279">
+        <v>4</v>
+      </c>
     </row>
     <row r="280">
       <c r="A280" t="inlineStr">
@@ -28678,6 +29517,9 @@
       <c r="AD280">
         <v>43</v>
       </c>
+      <c r="AE280">
+        <v>48</v>
+      </c>
     </row>
     <row r="281">
       <c r="A281" t="inlineStr">
@@ -28778,6 +29620,9 @@
       <c r="AD281">
         <v>30</v>
       </c>
+      <c r="AE281">
+        <v>31</v>
+      </c>
     </row>
     <row r="282">
       <c r="A282" t="inlineStr">
@@ -28878,6 +29723,9 @@
       <c r="AD282">
         <v>1</v>
       </c>
+      <c r="AE282">
+        <v>1</v>
+      </c>
     </row>
     <row r="283">
       <c r="A283" t="inlineStr">
@@ -28978,6 +29826,9 @@
       <c r="AD283">
         <v>0</v>
       </c>
+      <c r="AE283">
+        <v>0</v>
+      </c>
     </row>
     <row r="284">
       <c r="A284" t="inlineStr">
@@ -29078,6 +29929,9 @@
       <c r="AD284">
         <v>9</v>
       </c>
+      <c r="AE284">
+        <v>20</v>
+      </c>
     </row>
     <row r="285">
       <c r="A285" t="inlineStr">
@@ -29178,6 +30032,9 @@
       <c r="AD285">
         <v>19</v>
       </c>
+      <c r="AE285">
+        <v>21</v>
+      </c>
     </row>
     <row r="286">
       <c r="A286" t="inlineStr">
@@ -29278,6 +30135,9 @@
       <c r="AD286">
         <v>0</v>
       </c>
+      <c r="AE286">
+        <v>0</v>
+      </c>
     </row>
     <row r="287">
       <c r="A287" t="inlineStr">
@@ -29378,6 +30238,9 @@
       <c r="AD287">
         <v>0</v>
       </c>
+      <c r="AE287">
+        <v>0</v>
+      </c>
     </row>
     <row r="288">
       <c r="A288" t="inlineStr">
@@ -29478,6 +30341,9 @@
       <c r="AD288">
         <v>0</v>
       </c>
+      <c r="AE288">
+        <v>0</v>
+      </c>
     </row>
     <row r="289">
       <c r="A289" t="inlineStr">
@@ -29578,6 +30444,9 @@
       <c r="AD289">
         <v>0</v>
       </c>
+      <c r="AE289">
+        <v>0</v>
+      </c>
     </row>
     <row r="290">
       <c r="A290" t="inlineStr">
@@ -29678,6 +30547,9 @@
       <c r="AD290">
         <v>3</v>
       </c>
+      <c r="AE290">
+        <v>3</v>
+      </c>
     </row>
     <row r="291">
       <c r="A291" t="inlineStr">
@@ -29778,6 +30650,9 @@
       <c r="AD291">
         <v>0</v>
       </c>
+      <c r="AE291">
+        <v>0</v>
+      </c>
     </row>
     <row r="292">
       <c r="A292" t="inlineStr">
@@ -29878,6 +30753,9 @@
       <c r="AD292">
         <v>3</v>
       </c>
+      <c r="AE292">
+        <v>3</v>
+      </c>
     </row>
     <row r="293">
       <c r="A293" t="inlineStr">
@@ -29978,6 +30856,9 @@
       <c r="AD293">
         <v>0</v>
       </c>
+      <c r="AE293">
+        <v>0</v>
+      </c>
     </row>
     <row r="294">
       <c r="A294" t="inlineStr">
@@ -30078,6 +30959,9 @@
       <c r="AD294">
         <v>7</v>
       </c>
+      <c r="AE294">
+        <v>7</v>
+      </c>
     </row>
     <row r="295">
       <c r="A295" t="inlineStr">
@@ -30178,6 +31062,9 @@
       <c r="AD295">
         <v>0</v>
       </c>
+      <c r="AE295">
+        <v>0</v>
+      </c>
     </row>
     <row r="296">
       <c r="A296" t="inlineStr">
@@ -30278,6 +31165,9 @@
       <c r="AD296">
         <v>0</v>
       </c>
+      <c r="AE296">
+        <v>0</v>
+      </c>
     </row>
     <row r="297">
       <c r="A297" t="inlineStr">
@@ -30378,6 +31268,9 @@
       <c r="AD297">
         <v>1</v>
       </c>
+      <c r="AE297">
+        <v>1</v>
+      </c>
     </row>
     <row r="298">
       <c r="A298" t="inlineStr">
@@ -30478,6 +31371,9 @@
       <c r="AD298">
         <v>4</v>
       </c>
+      <c r="AE298">
+        <v>4</v>
+      </c>
     </row>
     <row r="299">
       <c r="A299" t="inlineStr">
@@ -30578,6 +31474,9 @@
       <c r="AD299">
         <v>0</v>
       </c>
+      <c r="AE299">
+        <v>0</v>
+      </c>
     </row>
     <row r="300">
       <c r="A300" t="inlineStr">
@@ -30678,6 +31577,9 @@
       <c r="AD300">
         <v>0</v>
       </c>
+      <c r="AE300">
+        <v>0</v>
+      </c>
     </row>
     <row r="301">
       <c r="A301" t="inlineStr">
@@ -30778,6 +31680,9 @@
       <c r="AD301">
         <v>17</v>
       </c>
+      <c r="AE301">
+        <v>17</v>
+      </c>
     </row>
     <row r="302">
       <c r="A302" t="inlineStr">
@@ -30878,6 +31783,9 @@
       <c r="AD302">
         <v>0</v>
       </c>
+      <c r="AE302">
+        <v>0</v>
+      </c>
     </row>
     <row r="303">
       <c r="A303" t="inlineStr">
@@ -30978,6 +31886,9 @@
       <c r="AD303">
         <v>0</v>
       </c>
+      <c r="AE303">
+        <v>0</v>
+      </c>
     </row>
     <row r="304">
       <c r="A304" t="inlineStr">
@@ -31078,6 +31989,9 @@
       <c r="AD304">
         <v>4</v>
       </c>
+      <c r="AE304">
+        <v>4</v>
+      </c>
     </row>
     <row r="305">
       <c r="A305" t="inlineStr">
@@ -31178,6 +32092,9 @@
       <c r="AD305">
         <v>12</v>
       </c>
+      <c r="AE305">
+        <v>12</v>
+      </c>
     </row>
     <row r="306">
       <c r="A306" t="inlineStr">
@@ -31278,6 +32195,9 @@
       <c r="AD306">
         <v>214</v>
       </c>
+      <c r="AE306">
+        <v>216</v>
+      </c>
     </row>
     <row r="307">
       <c r="A307" t="inlineStr">
@@ -31378,6 +32298,9 @@
       <c r="AD307">
         <v>16</v>
       </c>
+      <c r="AE307">
+        <v>16</v>
+      </c>
     </row>
     <row r="308">
       <c r="A308" t="inlineStr">
@@ -31478,6 +32401,9 @@
       <c r="AD308">
         <v>5</v>
       </c>
+      <c r="AE308">
+        <v>5</v>
+      </c>
     </row>
     <row r="309">
       <c r="A309" t="inlineStr">
@@ -31578,6 +32504,9 @@
       <c r="AD309">
         <v>0</v>
       </c>
+      <c r="AE309">
+        <v>0</v>
+      </c>
     </row>
     <row r="310">
       <c r="A310" t="inlineStr">
@@ -31678,6 +32607,9 @@
       <c r="AD310">
         <v>0</v>
       </c>
+      <c r="AE310">
+        <v>0</v>
+      </c>
     </row>
     <row r="311">
       <c r="A311" t="inlineStr">
@@ -31778,6 +32710,9 @@
       <c r="AD311">
         <v>8</v>
       </c>
+      <c r="AE311">
+        <v>8</v>
+      </c>
     </row>
     <row r="312">
       <c r="A312" t="inlineStr">
@@ -31878,6 +32813,9 @@
       <c r="AD312">
         <v>5</v>
       </c>
+      <c r="AE312">
+        <v>5</v>
+      </c>
     </row>
     <row r="313">
       <c r="A313" t="inlineStr">
@@ -31978,6 +32916,9 @@
       <c r="AD313">
         <v>0</v>
       </c>
+      <c r="AE313">
+        <v>0</v>
+      </c>
     </row>
     <row r="314">
       <c r="A314" t="inlineStr">
@@ -32078,6 +33019,9 @@
       <c r="AD314">
         <v>1</v>
       </c>
+      <c r="AE314">
+        <v>1</v>
+      </c>
     </row>
     <row r="315">
       <c r="A315" t="inlineStr">
@@ -32178,6 +33122,9 @@
       <c r="AD315">
         <v>7</v>
       </c>
+      <c r="AE315">
+        <v>7</v>
+      </c>
     </row>
     <row r="316">
       <c r="A316" t="inlineStr">
@@ -32278,6 +33225,9 @@
       <c r="AD316">
         <v>3</v>
       </c>
+      <c r="AE316">
+        <v>3</v>
+      </c>
     </row>
     <row r="317">
       <c r="A317" t="inlineStr">
@@ -32378,6 +33328,9 @@
       <c r="AD317">
         <v>5</v>
       </c>
+      <c r="AE317">
+        <v>5</v>
+      </c>
     </row>
     <row r="318">
       <c r="A318" t="inlineStr">
@@ -32478,6 +33431,9 @@
       <c r="AD318">
         <v>11</v>
       </c>
+      <c r="AE318">
+        <v>11</v>
+      </c>
     </row>
     <row r="319">
       <c r="A319" t="inlineStr">
@@ -32578,6 +33534,9 @@
       <c r="AD319">
         <v>6</v>
       </c>
+      <c r="AE319">
+        <v>6</v>
+      </c>
     </row>
     <row r="320">
       <c r="A320" t="inlineStr">
@@ -32678,6 +33637,9 @@
       <c r="AD320">
         <v>0</v>
       </c>
+      <c r="AE320">
+        <v>0</v>
+      </c>
     </row>
     <row r="321">
       <c r="A321" t="inlineStr">
@@ -32778,6 +33740,9 @@
       <c r="AD321">
         <v>1</v>
       </c>
+      <c r="AE321">
+        <v>1</v>
+      </c>
     </row>
     <row r="322">
       <c r="A322" t="inlineStr">
@@ -32878,6 +33843,9 @@
       <c r="AD322">
         <v>7</v>
       </c>
+      <c r="AE322">
+        <v>7</v>
+      </c>
     </row>
     <row r="323">
       <c r="A323" t="inlineStr">
@@ -32978,6 +33946,9 @@
       <c r="AD323">
         <v>28</v>
       </c>
+      <c r="AE323">
+        <v>28</v>
+      </c>
     </row>
     <row r="324">
       <c r="A324" t="inlineStr">
@@ -33078,6 +34049,9 @@
       <c r="AD324">
         <v>21</v>
       </c>
+      <c r="AE324">
+        <v>21</v>
+      </c>
     </row>
     <row r="325">
       <c r="A325" t="inlineStr">
@@ -33178,6 +34152,9 @@
       <c r="AD325">
         <v>15</v>
       </c>
+      <c r="AE325">
+        <v>15</v>
+      </c>
     </row>
     <row r="326">
       <c r="A326" t="inlineStr">
@@ -33278,6 +34255,9 @@
       <c r="AD326">
         <v>0</v>
       </c>
+      <c r="AE326">
+        <v>0</v>
+      </c>
     </row>
     <row r="327">
       <c r="A327" t="inlineStr">
@@ -33378,6 +34358,9 @@
       <c r="AD327">
         <v>0</v>
       </c>
+      <c r="AE327">
+        <v>0</v>
+      </c>
     </row>
     <row r="328">
       <c r="A328" t="inlineStr">
@@ -33478,6 +34461,9 @@
       <c r="AD328">
         <v>0</v>
       </c>
+      <c r="AE328">
+        <v>0</v>
+      </c>
     </row>
     <row r="329">
       <c r="A329" t="inlineStr">
@@ -33578,6 +34564,9 @@
       <c r="AD329">
         <v>0</v>
       </c>
+      <c r="AE329">
+        <v>0</v>
+      </c>
     </row>
     <row r="330">
       <c r="A330" t="inlineStr">
@@ -33678,6 +34667,9 @@
       <c r="AD330">
         <v>3</v>
       </c>
+      <c r="AE330">
+        <v>3</v>
+      </c>
     </row>
     <row r="331">
       <c r="A331" t="inlineStr">
@@ -33778,6 +34770,9 @@
       <c r="AD331">
         <v>1</v>
       </c>
+      <c r="AE331">
+        <v>1</v>
+      </c>
     </row>
     <row r="332">
       <c r="A332" t="inlineStr">
@@ -33878,6 +34873,9 @@
       <c r="AD332">
         <v>4</v>
       </c>
+      <c r="AE332">
+        <v>4</v>
+      </c>
     </row>
     <row r="333">
       <c r="A333" t="inlineStr">
@@ -33978,6 +34976,9 @@
       <c r="AD333">
         <v>0</v>
       </c>
+      <c r="AE333">
+        <v>0</v>
+      </c>
     </row>
     <row r="334">
       <c r="A334" t="inlineStr">
@@ -34078,6 +35079,9 @@
       <c r="AD334">
         <v>0</v>
       </c>
+      <c r="AE334">
+        <v>0</v>
+      </c>
     </row>
     <row r="335">
       <c r="A335" t="inlineStr">
@@ -34178,6 +35182,9 @@
       <c r="AD335">
         <v>7</v>
       </c>
+      <c r="AE335">
+        <v>7</v>
+      </c>
     </row>
     <row r="336">
       <c r="A336" t="inlineStr">
@@ -34278,6 +35285,9 @@
       <c r="AD336">
         <v>2</v>
       </c>
+      <c r="AE336">
+        <v>2</v>
+      </c>
     </row>
     <row r="337">
       <c r="A337" t="inlineStr">
@@ -34378,6 +35388,9 @@
       <c r="AD337">
         <v>2</v>
       </c>
+      <c r="AE337">
+        <v>2</v>
+      </c>
     </row>
     <row r="338">
       <c r="A338" t="inlineStr">
@@ -34478,6 +35491,9 @@
       <c r="AD338">
         <v>2</v>
       </c>
+      <c r="AE338">
+        <v>2</v>
+      </c>
     </row>
     <row r="339">
       <c r="A339" t="inlineStr">
@@ -34578,6 +35594,9 @@
       <c r="AD339">
         <v>10</v>
       </c>
+      <c r="AE339">
+        <v>10</v>
+      </c>
     </row>
     <row r="340">
       <c r="A340" t="inlineStr">
@@ -34678,6 +35697,9 @@
       <c r="AD340">
         <v>1</v>
       </c>
+      <c r="AE340">
+        <v>1</v>
+      </c>
     </row>
     <row r="341">
       <c r="A341" t="inlineStr">
@@ -34778,6 +35800,9 @@
       <c r="AD341">
         <v>17</v>
       </c>
+      <c r="AE341">
+        <v>17</v>
+      </c>
     </row>
     <row r="342">
       <c r="A342" t="inlineStr">
@@ -34878,6 +35903,9 @@
       <c r="AD342">
         <v>0</v>
       </c>
+      <c r="AE342">
+        <v>0</v>
+      </c>
     </row>
     <row r="343">
       <c r="A343" t="inlineStr">
@@ -34978,6 +36006,9 @@
       <c r="AD343">
         <v>0</v>
       </c>
+      <c r="AE343">
+        <v>0</v>
+      </c>
     </row>
     <row r="344">
       <c r="A344" t="inlineStr">
@@ -35078,6 +36109,9 @@
       <c r="AD344">
         <v>122</v>
       </c>
+      <c r="AE344">
+        <v>124</v>
+      </c>
     </row>
     <row r="345">
       <c r="A345" t="inlineStr">
@@ -35178,6 +36212,9 @@
       <c r="AD345">
         <v>4</v>
       </c>
+      <c r="AE345">
+        <v>4</v>
+      </c>
     </row>
     <row r="346">
       <c r="A346" t="inlineStr">
@@ -35278,6 +36315,9 @@
       <c r="AD346">
         <v>5</v>
       </c>
+      <c r="AE346">
+        <v>5</v>
+      </c>
     </row>
     <row r="347">
       <c r="A347" t="inlineStr">
@@ -35378,6 +36418,9 @@
       <c r="AD347">
         <v>1</v>
       </c>
+      <c r="AE347">
+        <v>1</v>
+      </c>
     </row>
     <row r="348">
       <c r="A348" t="inlineStr">
@@ -35478,6 +36521,9 @@
       <c r="AD348">
         <v>3</v>
       </c>
+      <c r="AE348">
+        <v>3</v>
+      </c>
     </row>
     <row r="349">
       <c r="A349" t="inlineStr">
@@ -35578,6 +36624,9 @@
       <c r="AD349">
         <v>14</v>
       </c>
+      <c r="AE349">
+        <v>14</v>
+      </c>
     </row>
     <row r="350">
       <c r="A350" t="inlineStr">
@@ -35678,6 +36727,9 @@
       <c r="AD350">
         <v>1</v>
       </c>
+      <c r="AE350">
+        <v>1</v>
+      </c>
     </row>
     <row r="351">
       <c r="A351" t="inlineStr">
@@ -35778,6 +36830,9 @@
       <c r="AD351">
         <v>1</v>
       </c>
+      <c r="AE351">
+        <v>1</v>
+      </c>
     </row>
     <row r="352">
       <c r="A352" t="inlineStr">
@@ -35878,6 +36933,9 @@
       <c r="AD352">
         <v>0</v>
       </c>
+      <c r="AE352">
+        <v>0</v>
+      </c>
     </row>
     <row r="353">
       <c r="A353" t="inlineStr">
@@ -35978,6 +37036,9 @@
       <c r="AD353">
         <v>0</v>
       </c>
+      <c r="AE353">
+        <v>0</v>
+      </c>
     </row>
     <row r="354">
       <c r="A354" t="inlineStr">
@@ -36078,6 +37139,9 @@
       <c r="AD354">
         <v>3</v>
       </c>
+      <c r="AE354">
+        <v>3</v>
+      </c>
     </row>
     <row r="355">
       <c r="A355" t="inlineStr">
@@ -36178,6 +37242,9 @@
       <c r="AD355">
         <v>1</v>
       </c>
+      <c r="AE355">
+        <v>1</v>
+      </c>
     </row>
     <row r="356">
       <c r="A356" t="inlineStr">
@@ -36278,6 +37345,9 @@
       <c r="AD356">
         <v>2</v>
       </c>
+      <c r="AE356">
+        <v>2</v>
+      </c>
     </row>
     <row r="357">
       <c r="A357" t="inlineStr">
@@ -36378,6 +37448,9 @@
       <c r="AD357">
         <v>0</v>
       </c>
+      <c r="AE357">
+        <v>0</v>
+      </c>
     </row>
     <row r="358">
       <c r="A358" t="inlineStr">
@@ -36478,6 +37551,9 @@
       <c r="AD358">
         <v>0</v>
       </c>
+      <c r="AE358">
+        <v>0</v>
+      </c>
     </row>
     <row r="359">
       <c r="A359" t="inlineStr">
@@ -36578,6 +37654,9 @@
       <c r="AD359">
         <v>0</v>
       </c>
+      <c r="AE359">
+        <v>0</v>
+      </c>
     </row>
     <row r="360">
       <c r="A360" t="inlineStr">
@@ -36678,6 +37757,9 @@
       <c r="AD360">
         <v>16</v>
       </c>
+      <c r="AE360">
+        <v>16</v>
+      </c>
     </row>
     <row r="361">
       <c r="A361" t="inlineStr">
@@ -36778,6 +37860,9 @@
       <c r="AD361">
         <v>2</v>
       </c>
+      <c r="AE361">
+        <v>2</v>
+      </c>
     </row>
     <row r="362">
       <c r="A362" t="inlineStr">
@@ -36878,6 +37963,9 @@
       <c r="AD362">
         <v>1</v>
       </c>
+      <c r="AE362">
+        <v>1</v>
+      </c>
     </row>
     <row r="363">
       <c r="A363" t="inlineStr">
@@ -36978,6 +38066,9 @@
       <c r="AD363">
         <v>2</v>
       </c>
+      <c r="AE363">
+        <v>2</v>
+      </c>
     </row>
     <row r="364">
       <c r="A364" t="inlineStr">
@@ -37078,6 +38169,9 @@
       <c r="AD364">
         <v>0</v>
       </c>
+      <c r="AE364">
+        <v>0</v>
+      </c>
     </row>
     <row r="365">
       <c r="A365" t="inlineStr">
@@ -37178,6 +38272,9 @@
       <c r="AD365">
         <v>0</v>
       </c>
+      <c r="AE365">
+        <v>0</v>
+      </c>
     </row>
     <row r="366">
       <c r="A366" t="inlineStr">
@@ -37278,6 +38375,9 @@
       <c r="AD366">
         <v>1</v>
       </c>
+      <c r="AE366">
+        <v>1</v>
+      </c>
     </row>
     <row r="367">
       <c r="A367" t="inlineStr">
@@ -37378,6 +38478,9 @@
       <c r="AD367">
         <v>2</v>
       </c>
+      <c r="AE367">
+        <v>2</v>
+      </c>
     </row>
     <row r="368">
       <c r="A368" t="inlineStr">
@@ -37478,6 +38581,9 @@
       <c r="AD368">
         <v>0</v>
       </c>
+      <c r="AE368">
+        <v>0</v>
+      </c>
     </row>
     <row r="369">
       <c r="A369" t="inlineStr">
@@ -37578,6 +38684,9 @@
       <c r="AD369">
         <v>1</v>
       </c>
+      <c r="AE369">
+        <v>1</v>
+      </c>
     </row>
     <row r="370">
       <c r="A370" t="inlineStr">
@@ -37678,6 +38787,9 @@
       <c r="AD370">
         <v>0</v>
       </c>
+      <c r="AE370">
+        <v>0</v>
+      </c>
     </row>
     <row r="371">
       <c r="A371" t="inlineStr">
@@ -37778,6 +38890,9 @@
       <c r="AD371">
         <v>0</v>
       </c>
+      <c r="AE371">
+        <v>0</v>
+      </c>
     </row>
     <row r="372">
       <c r="A372" t="inlineStr">
@@ -37878,6 +38993,9 @@
       <c r="AD372">
         <v>2</v>
       </c>
+      <c r="AE372">
+        <v>3</v>
+      </c>
     </row>
     <row r="373">
       <c r="A373" t="inlineStr">
@@ -37978,6 +39096,9 @@
       <c r="AD373">
         <v>2</v>
       </c>
+      <c r="AE373">
+        <v>2</v>
+      </c>
     </row>
     <row r="374">
       <c r="A374" t="inlineStr">
@@ -38078,6 +39199,9 @@
       <c r="AD374">
         <v>4</v>
       </c>
+      <c r="AE374">
+        <v>4</v>
+      </c>
     </row>
     <row r="375">
       <c r="A375" t="inlineStr">
@@ -38178,6 +39302,9 @@
       <c r="AD375">
         <v>1</v>
       </c>
+      <c r="AE375">
+        <v>1</v>
+      </c>
     </row>
     <row r="376">
       <c r="A376" t="inlineStr">
@@ -38278,6 +39405,9 @@
       <c r="AD376">
         <v>0</v>
       </c>
+      <c r="AE376">
+        <v>0</v>
+      </c>
     </row>
     <row r="377">
       <c r="A377" t="inlineStr">
@@ -38378,6 +39508,9 @@
       <c r="AD377">
         <v>0</v>
       </c>
+      <c r="AE377">
+        <v>0</v>
+      </c>
     </row>
     <row r="378">
       <c r="A378" t="inlineStr">
@@ -38478,6 +39611,9 @@
       <c r="AD378">
         <v>0</v>
       </c>
+      <c r="AE378">
+        <v>0</v>
+      </c>
     </row>
     <row r="379">
       <c r="A379" t="inlineStr">
@@ -38578,6 +39714,9 @@
       <c r="AD379">
         <v>1</v>
       </c>
+      <c r="AE379">
+        <v>1</v>
+      </c>
     </row>
     <row r="380">
       <c r="A380" t="inlineStr">
@@ -38678,6 +39817,9 @@
       <c r="AD380">
         <v>1</v>
       </c>
+      <c r="AE380">
+        <v>1</v>
+      </c>
     </row>
     <row r="381">
       <c r="A381" t="inlineStr">
@@ -38778,6 +39920,9 @@
       <c r="AD381">
         <v>0</v>
       </c>
+      <c r="AE381">
+        <v>0</v>
+      </c>
     </row>
     <row r="382">
       <c r="A382" t="inlineStr">
@@ -38878,6 +40023,9 @@
       <c r="AD382">
         <v>4</v>
       </c>
+      <c r="AE382">
+        <v>4</v>
+      </c>
     </row>
     <row r="383">
       <c r="A383" t="inlineStr">
@@ -38978,6 +40126,9 @@
       <c r="AD383">
         <v>0</v>
       </c>
+      <c r="AE383">
+        <v>0</v>
+      </c>
     </row>
     <row r="384">
       <c r="A384" t="inlineStr">
@@ -39076,6 +40227,9 @@
         <v>6</v>
       </c>
       <c r="AD384">
+        <v>7</v>
+      </c>
+      <c r="AE384">
         <v>7</v>
       </c>
     </row>

</xml_diff>